<commit_message>
Team - Nov 03
</commit_message>
<xml_diff>
--- a/Resources/Clean Data/Data Transformation Process and Plan.xlsx
+++ b/Resources/Clean Data/Data Transformation Process and Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e23db62feec2a5d/Desktop/U of T BootCamp/Homework/Unit 6 - Project 1/CanadaEnergyIE/Resources/Clean Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{669D6762-748D-4BB8-B1DA-CBBC129544A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32D696A1-E0C0-4093-86E9-7CAC7AC2A99E}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{669D6762-748D-4BB8-B1DA-CBBC129544A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{898B3386-8593-4836-951F-E88F0040A041}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9B33D0E1-F168-4917-B233-3C6CBB1CDC02}"/>
   </bookViews>
@@ -19,9 +19,6 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
-    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="114">
   <si>
     <t>Resources</t>
   </si>
@@ -413,6 +410,21 @@
   <si>
     <t>Key: 3ff2b2699c5d6a38b88da865b449afed</t>
   </si>
+  <si>
+    <t>Arima</t>
+  </si>
+  <si>
+    <t>https://www.machinelearningplus.com/time-series/arima-model-time-series-forecasting-python/#:~:text=So%20what%20exactly%20is%20an,used%20to%20forecast%20future%20values.</t>
+  </si>
+  <si>
+    <t>https://facebook.github.io/prophet/</t>
+  </si>
+  <si>
+    <t>Forecasting using ARIMA</t>
+  </si>
+  <si>
+    <t>(FB Profit is the library built in ARIMA, ARIMA is the model)</t>
+  </si>
 </sst>
 </file>
 
@@ -421,7 +433,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,10 +497,17 @@
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -611,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -646,45 +665,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -700,6 +680,47 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2170,7 +2191,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -2740,7 +2761,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$H$2:$H$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$H$2:$H$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -3557,7 +3578,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$B$1</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3590,7 +3611,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -4160,7 +4181,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$B$2:$B$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$B$2:$B$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -4740,7 +4761,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$C$1</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4773,7 +4794,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -5343,7 +5364,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$C$2:$C$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$C$2:$C$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -5923,7 +5944,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$D$1</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5956,7 +5977,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -6526,7 +6547,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$D$2:$D$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$D$2:$D$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -7106,7 +7127,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$E$1</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7139,7 +7160,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -7709,7 +7730,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$E$2:$E$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$E$2:$E$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -8289,7 +8310,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$F$1</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8322,7 +8343,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -8892,7 +8913,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$F$2:$F$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$F$2:$F$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -9472,7 +9493,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$G$1</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9505,7 +9526,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$A$2:$A$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -10075,7 +10096,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'[3]Renewable Energy (2005-2020)'!$G$2:$G$188</c:f>
+              <c:f>'[2]Renewable Energy (2005-2020)'!$G$2:$G$188</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="187"/>
@@ -12789,6 +12810,138 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>138546</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>221673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>671512</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>67849</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{042C04FF-F246-40A4-8652-C9E0FBFC792F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17830801" y="7439891"/>
+          <a:ext cx="4578493" cy="2755631"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>138546</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>566771</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>40140</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF7F7357-34F9-4A2F-9A5F-5A28158503A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6650182" y="10931236"/>
+          <a:ext cx="4584589" cy="2755631"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>539062</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>40140</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8D8D2EE-7D8C-4699-BF07-D118D6303F06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17692255" y="10931236"/>
+          <a:ext cx="4584589" cy="2755631"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -14194,19 +14347,6 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="CO-Type"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
       <sheetName val="Table 9 - US_electricity_net_ge"/>
       <sheetName val="Renewable Energy (2005-2020)"/>
     </sheetNames>
@@ -19096,153 +19236,6 @@
           </cell>
         </row>
       </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="share-electricity-renewables"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="867">
-          <cell r="C867">
-            <v>2005</v>
-          </cell>
-          <cell r="D867">
-            <v>59.701435018311301</v>
-          </cell>
-        </row>
-        <row r="868">
-          <cell r="C868">
-            <v>2006</v>
-          </cell>
-          <cell r="D868">
-            <v>59.523241425702402</v>
-          </cell>
-        </row>
-        <row r="869">
-          <cell r="C869">
-            <v>2007</v>
-          </cell>
-          <cell r="D869">
-            <v>59.586851373912197</v>
-          </cell>
-        </row>
-        <row r="870">
-          <cell r="C870">
-            <v>2008</v>
-          </cell>
-          <cell r="D870">
-            <v>61.2958829648557</v>
-          </cell>
-        </row>
-        <row r="871">
-          <cell r="C871">
-            <v>2009</v>
-          </cell>
-          <cell r="D871">
-            <v>62.611092629300799</v>
-          </cell>
-        </row>
-        <row r="872">
-          <cell r="C872">
-            <v>2010</v>
-          </cell>
-          <cell r="D872">
-            <v>61.066483611107401</v>
-          </cell>
-        </row>
-        <row r="873">
-          <cell r="C873">
-            <v>2011</v>
-          </cell>
-          <cell r="D873">
-            <v>62.150886714035799</v>
-          </cell>
-        </row>
-        <row r="874">
-          <cell r="C874">
-            <v>2012</v>
-          </cell>
-          <cell r="D874">
-            <v>63.369407000974</v>
-          </cell>
-        </row>
-        <row r="875">
-          <cell r="C875">
-            <v>2013</v>
-          </cell>
-          <cell r="D875">
-            <v>63.364457737178199</v>
-          </cell>
-        </row>
-        <row r="876">
-          <cell r="C876">
-            <v>2014</v>
-          </cell>
-          <cell r="D876">
-            <v>62.888119619547197</v>
-          </cell>
-        </row>
-        <row r="877">
-          <cell r="C877">
-            <v>2015</v>
-          </cell>
-          <cell r="D877">
-            <v>64.008832342385404</v>
-          </cell>
-        </row>
-        <row r="878">
-          <cell r="C878">
-            <v>2016</v>
-          </cell>
-          <cell r="D878">
-            <v>65.008523823952203</v>
-          </cell>
-        </row>
-        <row r="879">
-          <cell r="C879">
-            <v>2017</v>
-          </cell>
-          <cell r="D879">
-            <v>66.292794456162298</v>
-          </cell>
-        </row>
-        <row r="880">
-          <cell r="C880">
-            <v>2018</v>
-          </cell>
-          <cell r="D880">
-            <v>66.376988247923194</v>
-          </cell>
-        </row>
-        <row r="881">
-          <cell r="C881">
-            <v>2019</v>
-          </cell>
-          <cell r="D881">
-            <v>65.302617203062297</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Table 3 - US Dollar Index - 200"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -19545,10 +19538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC56270A-589E-410B-A871-469A984B00F0}">
-  <dimension ref="A1:AC49"/>
+  <dimension ref="A1:AC56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33"/>
+      <selection activeCell="U66" sqref="U66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19565,74 +19558,77 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="2" spans="1:29" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="26"/>
-      <c r="P2" s="20" t="s">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
+      <c r="P2" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="22"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="29"/>
     </row>
     <row r="3" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="P3" s="17" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="P3" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
-      <c r="X3" s="17"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="17"/>
-      <c r="AB3" s="17"/>
-      <c r="AC3" s="17"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
     </row>
     <row r="4" spans="1:29" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -19680,43 +19676,43 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="24"/>
       <c r="Q8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
       <c r="P9">
         <v>2</v>
       </c>
@@ -19725,131 +19721,131 @@
       </c>
     </row>
     <row r="10" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
       <c r="O10" s="10"/>
-      <c r="P10" s="20" t="s">
+      <c r="P10" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="22"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="29"/>
     </row>
     <row r="11" spans="1:29" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="32" t="s">
+      <c r="I11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="32" t="s">
+      <c r="J11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="32" t="s">
+      <c r="K11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="L11" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="32" t="s">
+      <c r="M11" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="32" t="s">
+      <c r="N11" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="P11" s="17" t="s">
+      <c r="P11" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="17"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="30"/>
+      <c r="S11" s="30"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="30"/>
+      <c r="X11" s="30"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="30"/>
+      <c r="AC11" s="30"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:29" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
       <c r="P13" s="12" t="s">
         <v>1</v>
       </c>
@@ -19890,67 +19886,67 @@
       <c r="AC13" s="12"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A14" s="30">
+      <c r="A14" s="17">
         <v>1</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A15" s="30">
+      <c r="A15" s="17">
         <v>2</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
       <c r="P15" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A16" s="30">
+      <c r="A16" s="17">
         <v>3</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
       <c r="P16">
         <v>1</v>
       </c>
@@ -19959,45 +19955,45 @@
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A17" s="30">
+      <c r="A17" s="17">
         <v>4</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
       <c r="P17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="21" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
       <c r="P18">
         <v>1</v>
       </c>
@@ -20006,22 +20002,22 @@
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
       <c r="P19">
         <v>2</v>
       </c>
@@ -20092,74 +20088,74 @@
       <c r="AC22" s="1"/>
     </row>
     <row r="23" spans="1:29" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="19" t="s">
+      <c r="P23" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
+      <c r="X23" s="35"/>
+      <c r="Y23" s="35"/>
+      <c r="Z23" s="35"/>
+      <c r="AA23" s="35"/>
+      <c r="AB23" s="35"/>
+      <c r="AC23" s="35"/>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="17" t="s">
+      <c r="P24" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="17"/>
-      <c r="V24" s="17"/>
-      <c r="W24" s="17"/>
-      <c r="X24" s="17"/>
-      <c r="Y24" s="17"/>
-      <c r="Z24" s="17"/>
-      <c r="AA24" s="17"/>
-      <c r="AB24" s="17"/>
-      <c r="AC24" s="17"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
+      <c r="AA24" s="30"/>
+      <c r="AB24" s="30"/>
+      <c r="AC24" s="30"/>
     </row>
     <row r="25" spans="1:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -20173,39 +20169,39 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="P26" s="30" t="s">
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="P26" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="Q26" s="30" t="s">
+      <c r="Q26" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
-      <c r="AA26" s="30"/>
-      <c r="AB26" s="30"/>
-      <c r="AC26" s="30"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="17"/>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B27" s="14"/>
@@ -20221,174 +20217,174 @@
       <c r="L27" s="14"/>
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
-      <c r="P27" s="30" t="s">
+      <c r="P27" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
-      <c r="U27" s="30"/>
-      <c r="V27" s="30"/>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="30"/>
-      <c r="AA27" s="30"/>
-      <c r="AB27" s="30"/>
-      <c r="AC27" s="30"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="P28" s="30">
+      <c r="P28" s="17">
         <v>1</v>
       </c>
-      <c r="Q28" s="30" t="s">
+      <c r="Q28" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="R28" s="30"/>
-      <c r="S28" s="30"/>
-      <c r="T28" s="30"/>
-      <c r="U28" s="30"/>
-      <c r="V28" s="30"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
-      <c r="Z28" s="30"/>
-      <c r="AA28" s="30"/>
-      <c r="AB28" s="30"/>
-      <c r="AC28" s="30"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B29" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="P29" s="30">
+      <c r="P29" s="17">
         <v>2</v>
       </c>
-      <c r="Q29" s="30" t="s">
+      <c r="Q29" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="R29" s="30"/>
-      <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="30"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="30"/>
-      <c r="X29" s="30"/>
-      <c r="Y29" s="30"/>
-      <c r="Z29" s="30"/>
-      <c r="AA29" s="30"/>
-      <c r="AB29" s="30"/>
-      <c r="AC29" s="30"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P30" s="30">
+      <c r="P30" s="17">
         <v>3</v>
       </c>
-      <c r="Q30" s="30" t="s">
+      <c r="Q30" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="R30" s="30"/>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="30"/>
-      <c r="Y30" s="30"/>
-      <c r="Z30" s="30"/>
-      <c r="AA30" s="30"/>
-      <c r="AB30" s="30"/>
-      <c r="AC30" s="30"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P31" s="30">
+      <c r="P31" s="17">
         <v>4</v>
       </c>
-      <c r="Q31" s="33" t="s">
+      <c r="Q31" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="30"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="30"/>
-      <c r="Z31" s="30"/>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="30"/>
-      <c r="AC31" s="30"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17"/>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="34" t="s">
+      <c r="P32" s="17"/>
+      <c r="Q32" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30" t="s">
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30"/>
-      <c r="AA32" s="30"/>
-      <c r="AB32" s="30"/>
-      <c r="AC32" s="30"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="34" t="s">
+      <c r="P33" s="17"/>
+      <c r="Q33" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="30"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="30"/>
-      <c r="Z33" s="30"/>
-      <c r="AA33" s="30"/>
-      <c r="AB33" s="30"/>
-      <c r="AC33" s="30"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="30"/>
-      <c r="AC34" s="30"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
     </row>
     <row r="35" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
@@ -20397,69 +20393,69 @@
       <c r="B35" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="P35" s="35" t="s">
+      <c r="P35" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="Q35" s="36" t="s">
+      <c r="Q35" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="R35" s="36" t="s">
+      <c r="R35" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
-      <c r="U35" s="30"/>
-      <c r="V35" s="30"/>
-      <c r="W35" s="30"/>
-      <c r="X35" s="30"/>
-      <c r="Y35" s="30"/>
-      <c r="Z35" s="30"/>
-      <c r="AA35" s="30"/>
-      <c r="AB35" s="30"/>
-      <c r="AC35" s="30"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="17"/>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30">
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17">
         <v>0.75</v>
       </c>
-      <c r="R36" s="30">
+      <c r="R36" s="17">
         <v>1</v>
       </c>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
-      <c r="Y36" s="30"/>
-      <c r="Z36" s="30"/>
-      <c r="AA36" s="30"/>
-      <c r="AB36" s="30"/>
-      <c r="AC36" s="30"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="17"/>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>49</v>
       </c>
-      <c r="P37" s="30"/>
-      <c r="Q37" s="30">
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17">
         <v>0.74</v>
       </c>
-      <c r="R37" s="30">
+      <c r="R37" s="17">
         <v>1</v>
       </c>
-      <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
-      <c r="U37" s="30"/>
-      <c r="V37" s="30"/>
-      <c r="W37" s="30"/>
-      <c r="X37" s="30"/>
-      <c r="Y37" s="30"/>
-      <c r="Z37" s="30"/>
-      <c r="AA37" s="30"/>
-      <c r="AB37" s="30"/>
-      <c r="AC37" s="30"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="17"/>
+      <c r="Y37" s="17"/>
+      <c r="Z37" s="17"/>
+      <c r="AA37" s="17"/>
+      <c r="AB37" s="17"/>
+      <c r="AC37" s="17"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -20484,74 +20480,74 @@
       <c r="AC38" s="1"/>
     </row>
     <row r="39" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
       <c r="O39" s="10"/>
-      <c r="P39" s="18" t="s">
+      <c r="P39" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
-      <c r="T39" s="18"/>
-      <c r="U39" s="18"/>
-      <c r="V39" s="18"/>
-      <c r="W39" s="18"/>
-      <c r="X39" s="18"/>
-      <c r="Y39" s="18"/>
-      <c r="Z39" s="18"/>
-      <c r="AA39" s="18"/>
-      <c r="AB39" s="18"/>
-      <c r="AC39" s="18"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+      <c r="AB39" s="26"/>
+      <c r="AC39" s="26"/>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="17"/>
-      <c r="M40" s="17"/>
-      <c r="N40" s="17"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
       <c r="O40" s="11"/>
-      <c r="P40" s="17" t="s">
+      <c r="P40" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="Q40" s="17"/>
-      <c r="R40" s="17"/>
-      <c r="S40" s="17"/>
-      <c r="T40" s="17"/>
-      <c r="U40" s="17"/>
-      <c r="V40" s="17"/>
-      <c r="W40" s="17"/>
-      <c r="X40" s="17"/>
-      <c r="Y40" s="17"/>
-      <c r="Z40" s="17"/>
-      <c r="AA40" s="17"/>
-      <c r="AB40" s="17"/>
-      <c r="AC40" s="17"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
+      <c r="S40" s="30"/>
+      <c r="T40" s="30"/>
+      <c r="U40" s="30"/>
+      <c r="V40" s="30"/>
+      <c r="W40" s="30"/>
+      <c r="X40" s="30"/>
+      <c r="Y40" s="30"/>
+      <c r="Z40" s="30"/>
+      <c r="AA40" s="30"/>
+      <c r="AB40" s="30"/>
+      <c r="AC40" s="30"/>
     </row>
     <row r="41" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
@@ -20648,11 +20644,85 @@
       <c r="AB48" s="1"/>
       <c r="AC48" s="1"/>
     </row>
-    <row r="49" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.3">
       <c r="O49" s="11"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B53" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="38"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B54" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="38"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B55" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="38"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B56" s="37" t="s">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A40:N40"/>
+    <mergeCell ref="P39:AC39"/>
+    <mergeCell ref="P40:AC40"/>
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="A24:N24"/>
+    <mergeCell ref="B26:N26"/>
+    <mergeCell ref="P24:AC24"/>
+    <mergeCell ref="A39:N39"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A9:N9"/>
     <mergeCell ref="A23:N23"/>
@@ -20663,15 +20733,6 @@
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="P23:AC23"/>
-    <mergeCell ref="A40:N40"/>
-    <mergeCell ref="P39:AC39"/>
-    <mergeCell ref="P40:AC40"/>
-    <mergeCell ref="A18:N18"/>
-    <mergeCell ref="A19:N19"/>
-    <mergeCell ref="A24:N24"/>
-    <mergeCell ref="B26:N26"/>
-    <mergeCell ref="P24:AC24"/>
-    <mergeCell ref="A39:N39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q32" r:id="rId1" xr:uid="{DB482FDF-A08F-441B-B744-36C17301768B}"/>

</xml_diff>